<commit_message>
removed temp files from tests
</commit_message>
<xml_diff>
--- a/tests/data/some_existing_ids.xlsx
+++ b/tests/data/some_existing_ids.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,62 +12,30 @@
     <sheet name="metadata" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
-    <font>
-      <name val="Calibri"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,19 +50,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -108,44 +72,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -172,32 +136,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -224,24 +170,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -253,142 +181,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -398,106 +350,106 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>variable</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>scenario</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>param</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>ref value</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>mean growth</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>initial_value_proportional_variation</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>variability growth</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>ref date</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>control</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>scenario notes</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>ui variable</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>user name</t>
         </is>
       </c>
-      <c r="S1" s="6" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -533,7 +485,7 @@
       <c r="H2" t="n">
         <v>0.05</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="1" t="n">
         <v>43617</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -541,17 +493,17 @@
           <t>W</t>
         </is>
       </c>
-      <c r="P2" s="3" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>what does it mean? How do collect this info?</t>
         </is>
       </c>
-      <c r="Q2" s="3" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="R2" s="3" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>power draw of laptop</t>
         </is>
@@ -590,7 +542,7 @@
       <c r="H3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="1" t="n">
         <v>43617</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -598,7 +550,7 @@
           <t>minute</t>
         </is>
       </c>
-      <c r="Q3" s="3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
@@ -627,7 +579,7 @@
       <c r="H4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="1" t="n">
         <v>42522</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -639,30 +591,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5">
-      <c r="E5" s="3" t="n"/>
-      <c r="I5" s="2" t="n"/>
-      <c r="J5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="I6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="I7" s="2" t="n"/>
-    </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="E9" s="3" t="n"/>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B1"/>
@@ -671,29 +608,29 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>31.7.18</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>DS change all to lowercase</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B1"/>
@@ -702,19 +639,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>